<commit_message>
`Binary files a/test.xlsx and b/test.xlsx differ`
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel Olabode\Documents\personal projects\CoinCoach\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7798BE-422D-488D-80FE-8D27C58392EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E23E30-2F4A-4FCF-BE42-4A7CA1806240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,36 +25,81 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>expense</t>
   </si>
   <si>
-    <t>grocieries</t>
-  </si>
-  <si>
-    <t>food</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>electronics</t>
-  </si>
-  <si>
     <t>income</t>
   </si>
   <si>
-    <t>job</t>
-  </si>
-  <si>
-    <t>my day job at Amazon</t>
-  </si>
-  <si>
-    <t>startup income</t>
-  </si>
-  <si>
-    <t>my app on play store is bringing in income</t>
+    <t>type</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Need to eat</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>My food expenses</t>
+  </si>
+  <si>
+    <t>salary</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>Day job pay every month</t>
+  </si>
+  <si>
+    <t>my pay</t>
+  </si>
+  <si>
+    <t>bought something in the store</t>
+  </si>
+  <si>
+    <t>sold my former laptop</t>
+  </si>
+  <si>
+    <t>sale</t>
+  </si>
+  <si>
+    <t>purchase</t>
+  </si>
+  <si>
+    <t>a new laptop</t>
+  </si>
+  <si>
+    <t>bought a new laptop</t>
+  </si>
+  <si>
+    <t>from startup</t>
+  </si>
+  <si>
+    <t>money from all my SAAS projects</t>
+  </si>
+  <si>
+    <t>a new monitor</t>
+  </si>
+  <si>
+    <t>sold my former monitor</t>
   </si>
 </sst>
 </file>
@@ -373,37 +418,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
-        <v>45997</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>25.5</v>
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>45942</v>
+        <v>46003</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -412,44 +465,141 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>2000</v>
+        <v>230</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>45629</v>
+        <v>45999</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D3">
-        <v>5000</v>
+        <v>5556</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>45970</v>
+        <v>45995</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D4">
-        <v>6000</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>45942</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>1200</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>45756</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>2300</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>46012</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>1200000</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>45711</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>129</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>45795</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>123</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
`Added recurring and recurrence fields to bulk upload and updated test.xlsx`
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel Olabode\Documents\personal projects\CoinCoach\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DABFD2-5D4C-4A02-95BF-7B0DEC8AB59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614E4180-C56F-4DC4-BC12-4BF41FF34E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>expense</t>
   </si>
@@ -100,6 +100,21 @@
   </si>
   <si>
     <t>sold my former monitor</t>
+  </si>
+  <si>
+    <t>recurring</t>
+  </si>
+  <si>
+    <t>recurrence</t>
+  </si>
+  <si>
+    <t>weekly</t>
+  </si>
+  <si>
+    <t>monthly</t>
+  </si>
+  <si>
+    <t>daily</t>
   </si>
 </sst>
 </file>
@@ -418,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,9 +447,10 @@
     <col min="4" max="4" width="17.88671875" customWidth="1"/>
     <col min="5" max="5" width="30.6640625" customWidth="1"/>
     <col min="6" max="6" width="27.21875" customWidth="1"/>
+    <col min="7" max="7" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -453,8 +469,14 @@
       <c r="F1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>46003</v>
       </c>
@@ -473,8 +495,14 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>45999</v>
       </c>
@@ -493,8 +521,14 @@
       <c r="F3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>45995</v>
       </c>
@@ -510,8 +544,11 @@
       <c r="F4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45942</v>
       </c>
@@ -527,8 +564,11 @@
       <c r="F5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>45756</v>
       </c>
@@ -547,8 +587,11 @@
       <c r="F6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>46012</v>
       </c>
@@ -567,8 +610,14 @@
       <c r="F7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>45711</v>
       </c>
@@ -584,8 +633,11 @@
       <c r="F8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>45795</v>
       </c>
@@ -600,6 +652,9 @@
       </c>
       <c r="F9" t="s">
         <v>24</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing bugs in the app codebase
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel Olabode\Documents\personal projects\CoinCoach\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614E4180-C56F-4DC4-BC12-4BF41FF34E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55480C24-89B6-4E71-AC66-AEDF93D6FFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13728" yWindow="0" windowWidth="9408" windowHeight="13056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>expense</t>
   </si>
@@ -39,9 +39,6 @@
     <t>amount</t>
   </si>
   <si>
-    <t>Food</t>
-  </si>
-  <si>
     <t>Need to eat</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t>salary</t>
   </si>
   <si>
-    <t>mm</t>
-  </si>
-  <si>
     <t>Day job pay every month</t>
   </si>
   <si>
@@ -78,21 +72,12 @@
     <t>sold my former laptop</t>
   </si>
   <si>
-    <t>sale</t>
-  </si>
-  <si>
-    <t>purchase</t>
-  </si>
-  <si>
     <t>a new laptop</t>
   </si>
   <si>
     <t>bought a new laptop</t>
   </si>
   <si>
-    <t>from startup</t>
-  </si>
-  <si>
     <t>money from all my SAAS projects</t>
   </si>
   <si>
@@ -115,6 +100,15 @@
   </si>
   <si>
     <t>daily</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>food</t>
+  </si>
+  <si>
+    <t>shopping</t>
   </si>
 </sst>
 </file>
@@ -435,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,28 +446,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -484,22 +478,22 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D2">
         <v>230</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -510,22 +504,22 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>5556</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -536,13 +530,13 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D4">
         <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G4" t="b">
         <v>0</v>
@@ -556,13 +550,13 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>1200</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -576,16 +570,16 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D6">
         <v>2300</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
@@ -599,22 +593,22 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>1200000</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -625,13 +619,13 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D8">
         <v>129</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
@@ -645,13 +639,13 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D9">
         <v>123</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>

</xml_diff>